<commit_message>
fix: tolerate empty columns in tabular files
</commit_message>
<xml_diff>
--- a/test/resources/datasets/actions.xlsx
+++ b/test/resources/datasets/actions.xlsx
@@ -149,50 +149,60 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>